<commit_message>
Ajout disclaimer et loading
</commit_message>
<xml_diff>
--- a/storage/app/public/input data/caseloads/lcb.xlsx
+++ b/storage/app/public/input data/caseloads/lcb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitednations.sharepoint.com/sites/OCHAROWCA/Information Management/30 DataBase/datas/caseloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{66F7D6D2-6BD9-45BA-A62C-684463D9957D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F599665-AE21-4CBF-9A2E-BB59F84668E9}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{66F7D6D2-6BD9-45BA-A62C-684463D9957D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{253F018A-304F-49D7-8B07-1DA67E5EA87D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2688" windowWidth="23040" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="156" yWindow="1536" windowWidth="22884" windowHeight="10188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="32">
   <si>
     <t>Country</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Tchad</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>HRP</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,10 @@
     <cellStyle name="Milliers [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -276,16 +285,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED10DA4E-D105-481B-ACFC-A68C22FCFC16}" name="Tableau1" displayName="Tableau1" ref="A1:J37" totalsRowShown="0">
-  <autoFilter ref="A1:J37" xr:uid="{3464EA4F-FC43-4D04-8195-39A8D46F9942}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Extreme-Nord"/>
-        <filter val="Extrême-Nord"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ED10DA4E-D105-481B-ACFC-A68C22FCFC16}" name="Tableau1" displayName="Tableau1" ref="A1:K37" totalsRowShown="0">
+  <autoFilter ref="A1:K37" xr:uid="{3464EA4F-FC43-4D04-8195-39A8D46F9942}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{594076F3-52C5-4F4D-87D8-6757CB8DC572}" name="Country"/>
     <tableColumn id="2" xr3:uid="{CBF2065D-E791-43E6-ABC3-D697932CF83D}" name="Country_Iso3"/>
     <tableColumn id="3" xr3:uid="{BC3628CE-440E-49D9-81CC-C6E40657BE21}" name="Admin1_name"/>
@@ -295,7 +297,8 @@
     <tableColumn id="7" xr3:uid="{9FB4AA86-862C-4650-9E74-E6F8AB7C5B02}" name="People_in_need"/>
     <tableColumn id="8" xr3:uid="{6A669401-7064-442C-B28C-63A9FF0888F1}" name="People_targeted"/>
     <tableColumn id="9" xr3:uid="{025746CC-F599-4DAC-A9D7-4C294979CDD2}" name="People_reached"/>
-    <tableColumn id="10" xr3:uid="{FEA66360-662B-40D7-A391-58CB1ADA1AFF}" name="Date" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{FEA66360-662B-40D7-A391-58CB1ADA1AFF}" name="Date" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{59137878-38F2-4E5A-B3F4-CD7C13000837}" name="Source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,10 +607,11 @@
     <col min="7" max="7" width="16.44140625" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,8 +642,11 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -670,8 +677,11 @@
       <c r="J2" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -702,8 +712,11 @@
       <c r="J3" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -734,8 +747,11 @@
       <c r="J4" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -766,8 +782,11 @@
       <c r="J5" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -798,8 +817,11 @@
       <c r="J6" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -830,8 +852,11 @@
       <c r="J7" s="1">
         <v>43754</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -853,8 +878,11 @@
       <c r="J8" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -876,8 +904,11 @@
       <c r="J9" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -899,8 +930,11 @@
       <c r="J10" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -918,8 +952,11 @@
       <c r="J11" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -937,8 +974,11 @@
       <c r="J12" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -960,8 +1000,11 @@
       <c r="J13" s="1">
         <v>44011</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -983,8 +1026,11 @@
       <c r="J14" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1006,8 +1052,11 @@
       <c r="J15" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1029,8 +1078,11 @@
       <c r="J16" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1048,8 +1100,11 @@
       <c r="J17" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1067,8 +1122,11 @@
       <c r="J18" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1090,8 +1148,11 @@
       <c r="J19" s="1">
         <v>44088</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1113,8 +1174,11 @@
       <c r="J20" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1136,8 +1200,11 @@
       <c r="J21" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1159,8 +1226,11 @@
       <c r="J22" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1178,8 +1248,11 @@
       <c r="J23" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1197,8 +1270,11 @@
       <c r="J24" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1220,8 +1296,11 @@
       <c r="J25" s="1">
         <v>44158</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1243,8 +1322,11 @@
       <c r="J26" s="1">
         <v>44222</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1266,8 +1348,11 @@
       <c r="J27" s="1">
         <v>44222</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1289,8 +1374,11 @@
       <c r="J28" s="1">
         <v>44270</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1312,8 +1400,11 @@
       <c r="J29" s="1">
         <v>44270</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1335,8 +1426,11 @@
       <c r="J30" s="1">
         <v>44270</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1358,8 +1452,11 @@
       <c r="J31" s="1">
         <v>44222</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1381,8 +1478,11 @@
       <c r="J32" s="1">
         <v>44278</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1404,8 +1504,11 @@
       <c r="J33" s="1">
         <v>44278</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1427,8 +1530,11 @@
       <c r="J34" s="1">
         <v>44278</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1450,8 +1556,11 @@
       <c r="J35" s="1">
         <v>44278</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1473,8 +1582,11 @@
       <c r="J36" s="1">
         <v>44278</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1496,10 +1608,13 @@
       <c r="J37" s="1">
         <v>44278</v>
       </c>
+      <c r="K37" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J14:J19">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="lastMonth">
+    <cfRule type="timePeriod" dxfId="2" priority="1" timePeriod="lastMonth">
       <formula>AND(MONTH(J14)=MONTH(EDATE(TODAY(),0-1)),YEAR(J14)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1512,6 +1627,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D56D188CBA27BF43BA16AB0991F8810A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d74f8ed3820e849c6c24bebf382cead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d04cdad-faad-4bbc-9725-fbca26071bed" xmlns:ns3="d4bd7185-3ccc-47d5-be69-542fd420c7c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="92b3107f17917cdf1896d29dfba996e5" ns2:_="" ns3:_="">
     <xsd:import namespace="2d04cdad-faad-4bbc-9725-fbca26071bed"/>
@@ -1728,12 +1849,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1744,6 +1859,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B020AB-1979-4CF4-9578-9E7259496776}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FC77710-C21E-4982-A067-C0EB3387D213}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1762,15 +1886,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B020AB-1979-4CF4-9578-9E7259496776}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CA285DB-A149-401B-9228-2545A285123A}">
   <ds:schemaRefs>

</xml_diff>